<commit_message>
Atualização do Soft - "block"
</commit_message>
<xml_diff>
--- a/Cronograma/aula 8.xlsx
+++ b/Cronograma/aula 8.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Aula ES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\Pim-Enfermagem\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Especificação do Teste</t>
   </si>
@@ -141,9 +141,6 @@
   </si>
   <si>
     <t>Segurança do sistema quanto as dados e identificação.</t>
-  </si>
-  <si>
-    <t>Tabela na aula 8 - pag7</t>
   </si>
 </sst>
 </file>
@@ -187,13 +184,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -475,9 +475,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -490,35 +492,43 @@
     <col min="9" max="9" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="D1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="2"/>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -532,7 +542,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -546,7 +556,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -560,7 +570,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -568,7 +578,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -576,7 +586,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -584,7 +594,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -595,7 +605,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -603,62 +613,70 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:1" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:1" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:1" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:1" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:1" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:1" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>